<commit_message>
Improve lookup functions with blank cells
</commit_message>
<xml_diff>
--- a/tests/fixtures/lookup.xlsx
+++ b/tests/fixtures/lookup.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB6DF69-F48E-4D1C-829B-89F704A39A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BD67B5-858C-491E-B577-6E3E37974B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40125" yWindow="8085" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41055" yWindow="8835" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
+    <sheet name="LookupBlanks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Inputs</t>
   </si>
@@ -101,6 +102,12 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
   </si>
 </sst>
 </file>
@@ -1885,7 +1892,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="e">
-        <f t="shared" ref="B41:O42" si="24">CHOOSE(B$40,$B3,$C3, $D3, $E3, $F3, $G3, $H3, $I3, $J3, $K3, $L3, $M3)</f>
+        <f t="shared" ref="B41:O41" si="24">CHOOSE(B$40,$B3,$C3, $D3, $E3, $F3, $G3, $H3, $I3, $J3, $K3, $L3, $M3)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C41" t="e">
@@ -2062,4 +2069,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7F526E-5A10-4BE5-88B6-267CA29FD357}">
+  <dimension ref="A4:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="e">
+        <f t="shared" ref="D5:D12" si="0">VLOOKUP(C5,A$1:A$16,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" t="e">
+        <f t="shared" ref="E5:E12" si="1">MATCH(C5,A$1:A$16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" t="e">
+        <f t="shared" ref="F5:F12" si="2">LOOKUP(C5,A$1:A$16)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement INDEX() Reference form Add handling for missing references in INDIRECT() and OFFSET()
</commit_message>
<xml_diff>
--- a/tests/fixtures/lookup.xlsx
+++ b/tests/fixtures/lookup.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BD67B5-858C-491E-B577-6E3E37974B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018AE24A-CE81-470D-9CF8-A08FF84D9C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41055" yWindow="8835" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40125" yWindow="8085" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
     <sheet name="LookupBlanks" sheetId="2" r:id="rId2"/>
+    <sheet name="Offset" sheetId="3" r:id="rId3"/>
+    <sheet name="Index" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,8 +28,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Inputs</t>
   </si>
@@ -109,13 +133,66 @@
   <si>
     <t>LOOKUP</t>
   </si>
+  <si>
+    <t>Data Table</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Cols</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>&lt;- Leave this at B53</t>
+  </si>
+  <si>
+    <t>A50</t>
+  </si>
+  <si>
+    <t>Reference Form</t>
+  </si>
+  <si>
+    <t>Array Form</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,11 +220,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2250,4 +2336,2162 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539435CD-BC31-49BA-A2E7-1B338D3F7687}">
+  <dimension ref="A1:I54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="9" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <f>1+B2</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <f>1+C2</f>
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <f>1+D2</f>
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>1+E2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <f>5+B2</f>
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:F5" si="0">1+D3</f>
+        <v>9</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <f>5+B3</f>
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:D6" si="1">1+B4</f>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <f>5+B4</f>
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <f>5+B5</f>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E6" s="4">
+        <f>1+D6</f>
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4">
+        <f>1+F6</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">OFFSET(B$2:F$6,B10,C10,D10,E10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F11" ca="1">OFFSET(B$2:F$6,B11,C11,D11,E11)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">OFFSET(B$2:F$6,B12,C12,D12,E12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" cm="1">
+        <f t="array" aca="1" ref="F13" ca="1">OFFSET(B$2:F$6,B13,C13,D13,E13)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F14" ca="1">OFFSET(B$2:F$6,B14,C14,D14,E14)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F15" ca="1">OFFSET(B$2:F$6,B15,C15,D15,E15)</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">OFFSET(B$2:F$6,B16,C16,D16,E16)</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F17:F18" ca="1">OFFSET(B$2:F$6,B17,C17,D17,E17)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="4">
+        <f ca="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F19:G19" ca="1">OFFSET(B$2:F$6,B19,C19,D19,E19)</f>
+        <v>X</v>
+      </c>
+      <c r="G19" s="4">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F21:G22" ca="1">OFFSET(B$2:F$6,B21,C21,D21,E21)</f>
+        <v>X</v>
+      </c>
+      <c r="G21" s="4">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="4">
+        <f ca="1"/>
+        <v>12</v>
+      </c>
+      <c r="G22" s="4">
+        <f ca="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" cm="1">
+        <f t="array" aca="1" ref="F23:F24" ca="1">OFFSET(B$2:F$6,B23,C23,D23,E23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="4">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4" cm="1">
+        <f t="array" aca="1" ref="F25:G25" ca="1">OFFSET(B$2:F$6,B25,C25,D25,E25)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2</v>
+      </c>
+      <c r="F27" s="4" cm="1">
+        <f t="array" aca="1" ref="F27:G28" ca="1">OFFSET(B$2:F$6,B27,C27,D27,E27)</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="4">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <f ca="1"/>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="F29" s="4" cm="1">
+        <f t="array" aca="1" ref="F29:G30" ca="1">OFFSET(B$2:F$6,B29,C29,D29,E29)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="4" t="str">
+        <f ca="1"/>
+        <v>Data Table</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C31" s="4">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2</v>
+      </c>
+      <c r="F31" s="4" cm="1">
+        <f t="array" aca="1" ref="F31:G32" ca="1">OFFSET(B$2:F$6,B31,C31,D31,E31)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="4">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="G32" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2</v>
+      </c>
+      <c r="F33" s="4" cm="1">
+        <f t="array" aca="1" ref="F33:G34" ca="1">OFFSET(B$2:F$6,B33,C33,D33,E33)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <f ca="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="4" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G34" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2</v>
+      </c>
+      <c r="F35" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="F35:G36" ca="1">OFFSET(B$2:F$6,B35,C35,D35,E35)</f>
+        <v>25</v>
+      </c>
+      <c r="G35" s="4">
+        <f ca="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="4" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4" cm="1">
+        <f t="array" aca="1" ref="F37:H39" ca="1">OFFSET(B$2:F$6,B37,C37,D37,E37)</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="4">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H37" s="4">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="4">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="G38" s="4" t="str">
+        <f ca="1"/>
+        <v>X</v>
+      </c>
+      <c r="H38" s="4">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="4">
+        <f ca="1"/>
+        <v>11</v>
+      </c>
+      <c r="G39" s="4">
+        <f ca="1"/>
+        <v>12</v>
+      </c>
+      <c r="H39" s="4">
+        <f ca="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4">
+        <v>3</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3</v>
+      </c>
+      <c r="E40" s="4">
+        <v>3</v>
+      </c>
+      <c r="F40" s="4" cm="1">
+        <f t="array" aca="1" ref="F40:H42" ca="1">OFFSET(B$2:F$6,B40,C40,D40,E40)</f>
+        <v>19</v>
+      </c>
+      <c r="G40" s="4">
+        <f ca="1"/>
+        <v>20</v>
+      </c>
+      <c r="H40" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="4">
+        <f ca="1"/>
+        <v>24</v>
+      </c>
+      <c r="G41" s="4" t="str">
+        <f ca="1"/>
+        <v>25</v>
+      </c>
+      <c r="H41" s="4">
+        <f ca="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="4" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>2</v>
+      </c>
+      <c r="D43" s="4">
+        <v>3</v>
+      </c>
+      <c r="E43" s="4">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" cm="1">
+        <f t="array" aca="1" ref="F43:I45" ca="1">OFFSET(B$2:F$6,B43,C43,D43,E43)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="4" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F44" s="4">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="G44" s="4">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H44" s="4">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="I44" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="4">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="G45" s="4">
+        <f ca="1"/>
+        <v>9</v>
+      </c>
+      <c r="H45" s="4">
+        <f ca="1"/>
+        <v>10</v>
+      </c>
+      <c r="I45" s="4">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4">
+        <v>4</v>
+      </c>
+      <c r="F46" s="4" cm="1">
+        <f t="array" aca="1" ref="F46:I48" ca="1">OFFSET(B$2:F$6,B46,C46,D46,E46)</f>
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H46" s="4">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="I46" s="4">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="4">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="G47" s="4" t="str">
+        <f ca="1"/>
+        <v>X</v>
+      </c>
+      <c r="H47" s="4">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="I47" s="4">
+        <f ca="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F48" s="4">
+        <f ca="1"/>
+        <v>11</v>
+      </c>
+      <c r="G48" s="4">
+        <f ca="1"/>
+        <v>12</v>
+      </c>
+      <c r="H48" s="4">
+        <f ca="1"/>
+        <v>13</v>
+      </c>
+      <c r="I48" s="4">
+        <f ca="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="4" cm="1">
+        <f t="array" aca="1" ref="B50:C51" ca="1">INDIRECT("H47:I48")</f>
+        <v>8</v>
+      </c>
+      <c r="C50" s="4">
+        <f ca="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <f ca="1"/>
+        <v>13</v>
+      </c>
+      <c r="C51" s="4">
+        <f ca="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="B53" ca="1">INDIRECT(B54)</f>
+        <v>Indirect</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB59B48F-6B90-449D-A295-54EA5EA7A00F}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <f>1+B2</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <f>1+C2</f>
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <f>1+D2</f>
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>1+E2</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <f>5+B2</f>
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:F5" si="0">1+D3</f>
+        <v>9</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <f>5+B3</f>
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:D6" si="1">1+B4</f>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <f>5+B4</f>
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <f>5+B5</f>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E6" s="4">
+        <f>1+D6</f>
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4">
+        <f>1+F6</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11" t="e" cm="1">
+        <f t="array" ref="C11">INDEX($B$2:$F$6,$B11,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" t="e" cm="1">
+        <f t="array" ref="D11">INDEX($B$2:$F$6,$B11,D$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E11" t="e" cm="1">
+        <f t="array" ref="E11">INDEX($B$2:$F$6,$B11,E$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" t="e" cm="1">
+        <f t="array" ref="F11">INDEX($B$2:$F$6,$B11,F$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" t="e" cm="1">
+        <f t="array" ref="G11">INDEX($B$2:$F$6,$B11,G$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" t="e" cm="1">
+        <f t="array" ref="H11">INDEX($B$2:$F$6,$B11,H$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" t="e" cm="1">
+        <f t="array" ref="I11">INDEX($B$2:$F$6,$B11,I$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J11" t="e" cm="1">
+        <f t="array" ref="J11">INDEX($B$2:$F$6,$B11,J$10)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="e" cm="1">
+        <f t="array" ref="C12">INDEX($B$2:$F$6,$B12,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12">INDEX($B$2:$F$6,$B12,D$10)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12">INDEX($B$2:$F$6,$B12,E$10)</f>
+        <v>2</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" ref="F12">INDEX($B$2:$F$6,$B12,F$10)</f>
+        <v>3</v>
+      </c>
+      <c r="G12" cm="1">
+        <f t="array" ref="G12">INDEX($B$2:$F$6,$B12,G$10)</f>
+        <v>4</v>
+      </c>
+      <c r="H12" cm="1">
+        <f t="array" ref="H12">INDEX($B$2:$F$6,$B12,H$10)</f>
+        <v>5</v>
+      </c>
+      <c r="I12" t="e" cm="1">
+        <f t="array" ref="I12">INDEX($B$2:$F$6,$B12,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J12" cm="1">
+        <f t="array" ref="J12:N12">INDEX($B$2:$F$6,$B12,J$10)</f>
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="e" cm="1">
+        <f t="array" ref="C13">INDEX($B$2:$F$6,$B13,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" cm="1">
+        <f t="array" ref="D13">INDEX($B$2:$F$6,$B13,D$10)</f>
+        <v>6</v>
+      </c>
+      <c r="E13" t="str" cm="1">
+        <f t="array" ref="E13">INDEX($B$2:$F$6,$B13,E$10)</f>
+        <v>X</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" ref="F13">INDEX($B$2:$F$6,$B13,F$10)</f>
+        <v>8</v>
+      </c>
+      <c r="G13" cm="1">
+        <f t="array" ref="G13">INDEX($B$2:$F$6,$B13,G$10)</f>
+        <v>9</v>
+      </c>
+      <c r="H13" cm="1">
+        <f t="array" ref="H13">INDEX($B$2:$F$6,$B13,H$10)</f>
+        <v>10</v>
+      </c>
+      <c r="I13" t="e" cm="1">
+        <f t="array" ref="I13">INDEX($B$2:$F$6,$B13,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" cm="1">
+        <f t="array" ref="J13:N13">INDEX($B$2:$F$6,$B13,J$10)</f>
+        <v>6</v>
+      </c>
+      <c r="K13" t="str">
+        <v>X</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="e" cm="1">
+        <f t="array" ref="C14">INDEX($B$2:$F$6,$B14,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" cm="1">
+        <f t="array" ref="D14">INDEX($B$2:$F$6,$B14,D$10)</f>
+        <v>11</v>
+      </c>
+      <c r="E14" cm="1">
+        <f t="array" ref="E14">INDEX($B$2:$F$6,$B14,E$10)</f>
+        <v>12</v>
+      </c>
+      <c r="F14" cm="1">
+        <f t="array" ref="F14">INDEX($B$2:$F$6,$B14,F$10)</f>
+        <v>13</v>
+      </c>
+      <c r="G14" cm="1">
+        <f t="array" ref="G14">INDEX($B$2:$F$6,$B14,G$10)</f>
+        <v>14</v>
+      </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14">INDEX($B$2:$F$6,$B14,H$10)</f>
+        <v>15</v>
+      </c>
+      <c r="I14" t="e" cm="1">
+        <f t="array" ref="I14">INDEX($B$2:$F$6,$B14,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" cm="1">
+        <f t="array" ref="J14:N14">INDEX($B$2:$F$6,$B14,J$10)</f>
+        <v>11</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>13</v>
+      </c>
+      <c r="M14">
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="e" cm="1">
+        <f t="array" ref="C15">INDEX($B$2:$F$6,$B15,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" cm="1">
+        <f t="array" ref="D15">INDEX($B$2:$F$6,$B15,D$10)</f>
+        <v>16</v>
+      </c>
+      <c r="E15" cm="1">
+        <f t="array" ref="E15">INDEX($B$2:$F$6,$B15,E$10)</f>
+        <v>17</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15">INDEX($B$2:$F$6,$B15,F$10)</f>
+        <v>18</v>
+      </c>
+      <c r="G15" cm="1">
+        <f t="array" ref="G15">INDEX($B$2:$F$6,$B15,G$10)</f>
+        <v>19</v>
+      </c>
+      <c r="H15" cm="1">
+        <f t="array" ref="H15">INDEX($B$2:$F$6,$B15,H$10)</f>
+        <v>20</v>
+      </c>
+      <c r="I15" t="e" cm="1">
+        <f t="array" ref="I15">INDEX($B$2:$F$6,$B15,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15:N15">INDEX($B$2:$F$6,$B15,J$10)</f>
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>17</v>
+      </c>
+      <c r="L15">
+        <v>18</v>
+      </c>
+      <c r="M15">
+        <v>19</v>
+      </c>
+      <c r="N15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="e" cm="1">
+        <f t="array" ref="C16">INDEX($B$2:$F$6,$B16,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D16" cm="1">
+        <f t="array" ref="D16">INDEX($B$2:$F$6,$B16,D$10)</f>
+        <v>21</v>
+      </c>
+      <c r="E16" cm="1">
+        <f t="array" ref="E16">INDEX($B$2:$F$6,$B16,E$10)</f>
+        <v>22</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16">INDEX($B$2:$F$6,$B16,F$10)</f>
+        <v>23</v>
+      </c>
+      <c r="G16" cm="1">
+        <f t="array" ref="G16">INDEX($B$2:$F$6,$B16,G$10)</f>
+        <v>24</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16">INDEX($B$2:$F$6,$B16,H$10)</f>
+        <v>25</v>
+      </c>
+      <c r="I16" t="e" cm="1">
+        <f t="array" ref="I16">INDEX($B$2:$F$6,$B16,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J16" cm="1">
+        <f t="array" ref="J16:N16">INDEX($B$2:$F$6,$B16,J$10)</f>
+        <v>21</v>
+      </c>
+      <c r="K16">
+        <v>22</v>
+      </c>
+      <c r="L16">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>24</v>
+      </c>
+      <c r="N16" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="e" cm="1">
+        <f t="array" ref="C17">INDEX($B$2:$F$6,$B17,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D17" t="e" cm="1">
+        <f t="array" ref="D17">INDEX($B$2:$F$6,$B17,D$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E17" t="e" cm="1">
+        <f t="array" ref="E17">INDEX($B$2:$F$6,$B17,E$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F17" t="e" cm="1">
+        <f t="array" ref="F17">INDEX($B$2:$F$6,$B17,F$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G17" t="e" cm="1">
+        <f t="array" ref="G17">INDEX($B$2:$F$6,$B17,G$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H17" t="e" cm="1">
+        <f t="array" ref="H17">INDEX($B$2:$F$6,$B17,H$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I17" t="e" cm="1">
+        <f t="array" ref="I17">INDEX($B$2:$F$6,$B17,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J17" t="e" cm="1">
+        <f t="array" ref="J17">INDEX($B$2:$F$6,$B17,J$10)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="e" cm="1">
+        <f t="array" ref="C18">INDEX($B$2:$F$6,$B18,C$10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" cm="1">
+        <f t="array" ref="D18:D22">INDEX($B$2:$F$6,$B18,D$10)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" cm="1">
+        <f t="array" ref="E18:E22">INDEX($B$2:$F$6,$B18,E$10)</f>
+        <v>2</v>
+      </c>
+      <c r="F18" cm="1">
+        <f t="array" ref="F18:F22">INDEX($B$2:$F$6,$B18,F$10)</f>
+        <v>3</v>
+      </c>
+      <c r="G18" cm="1">
+        <f t="array" ref="G18:G22">INDEX($B$2:$F$6,$B18,G$10)</f>
+        <v>4</v>
+      </c>
+      <c r="H18" cm="1">
+        <f t="array" ref="H18:H22">INDEX($B$2:$F$6,$B18,H$10)</f>
+        <v>5</v>
+      </c>
+      <c r="I18" t="e" cm="1">
+        <f t="array" ref="I18">INDEX($B$2:$F$6,$B18,I$10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J18" cm="1">
+        <f t="array" ref="J18:N22">INDEX($B$2:$F$6,$B18,J$10)</f>
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" t="str">
+        <v>X</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>9</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19" t="str">
+        <v>X</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+      <c r="J20">
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="L20">
+        <v>13</v>
+      </c>
+      <c r="M20">
+        <v>14</v>
+      </c>
+      <c r="N20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>17</v>
+      </c>
+      <c r="L21">
+        <v>18</v>
+      </c>
+      <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>23</v>
+      </c>
+      <c r="G22">
+        <v>24</v>
+      </c>
+      <c r="H22" t="str">
+        <v>25</v>
+      </c>
+      <c r="J22">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>22</v>
+      </c>
+      <c r="L22">
+        <v>23</v>
+      </c>
+      <c r="M22">
+        <v>24</v>
+      </c>
+      <c r="N22" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>-1</v>
+      </c>
+      <c r="C26" t="e" cm="1">
+        <f t="array" ref="C26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D26" t="e" cm="1">
+        <f t="array" ref="D26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,D$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E26" t="e" cm="1">
+        <f t="array" ref="E26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,E$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F26" t="e" cm="1">
+        <f t="array" ref="F26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,F$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G26" t="e" cm="1">
+        <f t="array" ref="G26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,G$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H26" t="e" cm="1">
+        <f t="array" ref="H26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,H$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I26" t="e" cm="1">
+        <f t="array" ref="I26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,I$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" t="e" cm="1">
+        <f t="array" ref="J26">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B26,J$25)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="e" cm="1">
+        <f t="array" ref="C27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D27" cm="1">
+        <f t="array" ref="D27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,D$25)</f>
+        <v>1</v>
+      </c>
+      <c r="E27" cm="1">
+        <f t="array" ref="E27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,E$25)</f>
+        <v>2</v>
+      </c>
+      <c r="F27" cm="1">
+        <f t="array" ref="F27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,F$25)</f>
+        <v>3</v>
+      </c>
+      <c r="G27" cm="1">
+        <f t="array" ref="G27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,G$25)</f>
+        <v>4</v>
+      </c>
+      <c r="H27" cm="1">
+        <f t="array" ref="H27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,H$25)</f>
+        <v>5</v>
+      </c>
+      <c r="I27" t="e" cm="1">
+        <f t="array" ref="I27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J27" cm="1">
+        <f t="array" ref="J27:N27">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B27,J$25)</f>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="e" cm="1">
+        <f t="array" ref="C28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D28" cm="1">
+        <f t="array" ref="D28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,D$25)</f>
+        <v>6</v>
+      </c>
+      <c r="E28" t="str" cm="1">
+        <f t="array" ref="E28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,E$25)</f>
+        <v>X</v>
+      </c>
+      <c r="F28" cm="1">
+        <f t="array" ref="F28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,F$25)</f>
+        <v>8</v>
+      </c>
+      <c r="G28" cm="1">
+        <f t="array" ref="G28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,G$25)</f>
+        <v>9</v>
+      </c>
+      <c r="H28" cm="1">
+        <f t="array" ref="H28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,H$25)</f>
+        <v>10</v>
+      </c>
+      <c r="I28" t="e" cm="1">
+        <f t="array" ref="I28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J28" cm="1">
+        <f t="array" ref="J28:N28">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B28,J$25)</f>
+        <v>6</v>
+      </c>
+      <c r="K28" t="str">
+        <v>X</v>
+      </c>
+      <c r="L28">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>9</v>
+      </c>
+      <c r="N28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="e" cm="1">
+        <f t="array" ref="C29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D29" cm="1">
+        <f t="array" ref="D29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,D$25)</f>
+        <v>11</v>
+      </c>
+      <c r="E29" cm="1">
+        <f t="array" ref="E29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,E$25)</f>
+        <v>12</v>
+      </c>
+      <c r="F29" cm="1">
+        <f t="array" ref="F29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,F$25)</f>
+        <v>13</v>
+      </c>
+      <c r="G29" cm="1">
+        <f t="array" ref="G29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,G$25)</f>
+        <v>14</v>
+      </c>
+      <c r="H29" cm="1">
+        <f t="array" ref="H29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,H$25)</f>
+        <v>15</v>
+      </c>
+      <c r="I29" t="e" cm="1">
+        <f t="array" ref="I29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J29" cm="1">
+        <f t="array" ref="J29:N29">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B29,J$25)</f>
+        <v>11</v>
+      </c>
+      <c r="K29">
+        <v>12</v>
+      </c>
+      <c r="L29">
+        <v>13</v>
+      </c>
+      <c r="M29">
+        <v>14</v>
+      </c>
+      <c r="N29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="e" cm="1">
+        <f t="array" ref="C30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D30" cm="1">
+        <f t="array" ref="D30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,D$25)</f>
+        <v>16</v>
+      </c>
+      <c r="E30" cm="1">
+        <f t="array" ref="E30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,E$25)</f>
+        <v>17</v>
+      </c>
+      <c r="F30" cm="1">
+        <f t="array" ref="F30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,F$25)</f>
+        <v>18</v>
+      </c>
+      <c r="G30" cm="1">
+        <f t="array" ref="G30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,G$25)</f>
+        <v>19</v>
+      </c>
+      <c r="H30" cm="1">
+        <f t="array" ref="H30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,H$25)</f>
+        <v>20</v>
+      </c>
+      <c r="I30" t="e" cm="1">
+        <f t="array" ref="I30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J30" cm="1">
+        <f t="array" ref="J30:N30">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B30,J$25)</f>
+        <v>16</v>
+      </c>
+      <c r="K30">
+        <v>17</v>
+      </c>
+      <c r="L30">
+        <v>18</v>
+      </c>
+      <c r="M30">
+        <v>19</v>
+      </c>
+      <c r="N30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="e" cm="1">
+        <f t="array" ref="C31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D31" cm="1">
+        <f t="array" ref="D31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,D$25)</f>
+        <v>21</v>
+      </c>
+      <c r="E31" cm="1">
+        <f t="array" ref="E31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,E$25)</f>
+        <v>22</v>
+      </c>
+      <c r="F31" cm="1">
+        <f t="array" ref="F31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,F$25)</f>
+        <v>23</v>
+      </c>
+      <c r="G31" cm="1">
+        <f t="array" ref="G31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,G$25)</f>
+        <v>24</v>
+      </c>
+      <c r="H31" t="str" cm="1">
+        <f t="array" ref="H31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,H$25)</f>
+        <v>25</v>
+      </c>
+      <c r="I31" t="e" cm="1">
+        <f t="array" ref="I31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J31" cm="1">
+        <f t="array" ref="J31:N31">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B31,J$25)</f>
+        <v>21</v>
+      </c>
+      <c r="K31">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <v>23</v>
+      </c>
+      <c r="M31">
+        <v>24</v>
+      </c>
+      <c r="N31" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="e" cm="1">
+        <f t="array" ref="C32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D32" t="e" cm="1">
+        <f t="array" ref="D32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,D$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E32" t="e" cm="1">
+        <f t="array" ref="E32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,E$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F32" t="e" cm="1">
+        <f t="array" ref="F32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,F$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G32" t="e" cm="1">
+        <f t="array" ref="G32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,G$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H32" t="e" cm="1">
+        <f t="array" ref="H32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,H$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I32" t="e" cm="1">
+        <f t="array" ref="I32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J32" t="e" cm="1">
+        <f t="array" ref="J32">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B32,J$25)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" t="e" cm="1">
+        <f t="array" ref="C33">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,C$25)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D33" cm="1">
+        <f t="array" ref="D33:D37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,D$25)</f>
+        <v>1</v>
+      </c>
+      <c r="E33" cm="1">
+        <f t="array" ref="E33:E37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,E$25)</f>
+        <v>2</v>
+      </c>
+      <c r="F33" cm="1">
+        <f t="array" ref="F33:F37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,F$25)</f>
+        <v>3</v>
+      </c>
+      <c r="G33" cm="1">
+        <f t="array" ref="G33:G37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,G$25)</f>
+        <v>4</v>
+      </c>
+      <c r="H33" cm="1">
+        <f t="array" ref="H33:H37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,H$25)</f>
+        <v>5</v>
+      </c>
+      <c r="I33" t="e" cm="1">
+        <f t="array" ref="I33">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,I$25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J33" cm="1">
+        <f t="array" ref="J33:N37">INDEX({1,2,3,4,5;6,"X",8,9,10;11,12,13,14,15;16,17,18,19,20;21,22,23,24,"25"},$B33,J$25)</f>
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>4</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" t="str">
+        <v>X</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34" t="str">
+        <v>X</v>
+      </c>
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>13</v>
+      </c>
+      <c r="G35">
+        <v>14</v>
+      </c>
+      <c r="H35">
+        <v>15</v>
+      </c>
+      <c r="J35">
+        <v>11</v>
+      </c>
+      <c r="K35">
+        <v>12</v>
+      </c>
+      <c r="L35">
+        <v>13</v>
+      </c>
+      <c r="M35">
+        <v>14</v>
+      </c>
+      <c r="N35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>19</v>
+      </c>
+      <c r="H36">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>16</v>
+      </c>
+      <c r="K36">
+        <v>17</v>
+      </c>
+      <c r="L36">
+        <v>18</v>
+      </c>
+      <c r="M36">
+        <v>19</v>
+      </c>
+      <c r="N36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>21</v>
+      </c>
+      <c r="E37">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <v>23</v>
+      </c>
+      <c r="G37">
+        <v>24</v>
+      </c>
+      <c r="H37" t="str">
+        <v>25</v>
+      </c>
+      <c r="J37">
+        <v>21</v>
+      </c>
+      <c r="K37">
+        <v>22</v>
+      </c>
+      <c r="L37">
+        <v>23</v>
+      </c>
+      <c r="M37">
+        <v>24</v>
+      </c>
+      <c r="N37" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>-1</v>
+      </c>
+      <c r="C40" t="e" cm="1">
+        <f t="array" ref="C40">INDEX({1,2;3,4},$B40)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G40">
+        <v>-1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" cm="1">
+        <f t="array" ref="C41:D41">INDEX({1,2;3,4},$B41)</f>
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="e" cm="1">
+        <f t="array" ref="G41">INDEX({1,2;3,4},,G$40)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H41" cm="1">
+        <f t="array" ref="H41:H42">INDEX({1,2;3,4},,H$40)</f>
+        <v>1</v>
+      </c>
+      <c r="I41" cm="1">
+        <f t="array" ref="I41:I42">INDEX({1,2;3,4},,I$40)</f>
+        <v>2</v>
+      </c>
+      <c r="J41" t="e" cm="1">
+        <f t="array" ref="J41">INDEX({1,2;3,4},,J$40)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K41" cm="1">
+        <f t="array" ref="K41:L42">INDEX({1,2;3,4},,K$40)</f>
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" cm="1">
+        <f t="array" ref="C42:D42">INDEX({1,2;3,4},$B42)</f>
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="e" cm="1">
+        <f t="array" ref="C43">INDEX({1,2;3,4},$B43)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" cm="1">
+        <f t="array" ref="C44:D45">INDEX({1,2;3,4},$B44)</f>
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>